<commit_message>
Cadastro, autenticação, reset de senha funcionando.
</commit_message>
<xml_diff>
--- a/projeto.xlsx
+++ b/projeto.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Páginas" sheetId="2" r:id="rId2"/>
+    <sheet name="Actions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
   <si>
     <t>Módulo</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>/user</t>
+  </si>
+  <si>
+    <t>Página</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Essa página vai mostrar um menu com opções. Usuário logado. Dashboard.</t>
   </si>
 </sst>
 </file>
@@ -158,6 +167,29 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Página"/>
+    <tableColumn id="2" name="Descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C2" totalsRowShown="0">
+  <autoFilter ref="A1:C2"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Página"/>
+    <tableColumn id="2" name="Controller"/>
+    <tableColumn id="3" name="Action"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="A4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,24 +700,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Autenticação funcionando como serviço.
</commit_message>
<xml_diff>
--- a/projeto.xlsx
+++ b/projeto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rotas" sheetId="4" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Plan1" sheetId="1" r:id="rId3"/>
     <sheet name="Páginas" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="76">
   <si>
     <t>Módulo</t>
   </si>
@@ -204,21 +204,9 @@
     <t>Formulário de edição.</t>
   </si>
   <si>
-    <t>Modificado</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-  <si>
     <t>Deleta o item selecionado.</t>
   </si>
   <si>
-    <t>Novo</t>
-  </si>
-  <si>
     <t>Resouces</t>
   </si>
   <si>
@@ -253,6 +241,15 @@
   </si>
   <si>
     <t>Mostra os dados do perfil do usuário.</t>
+  </si>
+  <si>
+    <t>Landing page.</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>Resource</t>
   </si>
 </sst>
 </file>
@@ -306,16 +303,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -344,16 +346,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:G23" totalsRowShown="0">
-  <autoFilter ref="A1:G23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:G28" totalsRowShown="0">
+  <autoFilter ref="A1:G28"/>
+  <sortState ref="A2:H24">
+    <sortCondition ref="A2:A24"/>
+    <sortCondition ref="B2:B24"/>
+    <sortCondition ref="C2:C24"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Module"/>
     <tableColumn id="2" name="Controller"/>
-    <tableColumn id="6" name="Extends"/>
     <tableColumn id="3" name="Action"/>
-    <tableColumn id="7" name="Modificado"/>
+    <tableColumn id="9" name="Extends"/>
     <tableColumn id="4" name="Parametros"/>
     <tableColumn id="5" name="Descrição"/>
+    <tableColumn id="8" name="Resource" dataDxfId="0">
+      <calculatedColumnFormula xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,7 +669,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,20 +818,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G28" sqref="G25:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -833,39 +846,40 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>Application\Controller\Index.index</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,22 +887,20 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="G3" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Privileges.add</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,19 +908,23 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Privileges.delete</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -916,22 +932,23 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
         <v>59</v>
+      </c>
+      <c r="G5" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Privileges.edit</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -939,19 +956,20 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Privileges.index</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -959,19 +977,20 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
         <v>58</v>
+      </c>
+      <c r="G7" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Resouces.add</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -979,22 +998,23 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="G8" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Resouces.delete</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1002,19 +1022,23 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Resouces.edit</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1022,22 +1046,20 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="G10" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Resouces.index</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,19 +1067,20 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Roles.add</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1065,22 +1088,23 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="G12" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Roles.delete</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1088,19 +1112,23 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Roles.edit</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1108,39 +1136,41 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="G14" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Roles.index</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilAcl\Controller\Roles.test</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1151,13 +1181,17 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Auth.login</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1165,16 +1199,20 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Auth.logout</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1185,13 +1223,20 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>70</v>
+      <c r="G18" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Index.activate</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1202,16 +1247,17 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="G19" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Index.forgot</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1222,10 +1268,17 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Index.index</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1236,16 +1289,17 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="G21" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Index.register</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1253,19 +1307,23 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Index.reset</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1273,19 +1331,134 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Profile.edit</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Profile.index</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="4" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Users.add</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="4" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Users.delete</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>14</v>
       </c>
-      <c r="E23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
         <v>51</v>
+      </c>
+      <c r="F27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="4" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Users.edit</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="4" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\Users.index</v>
       </c>
     </row>
   </sheetData>
@@ -1301,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modificações nas entidades do Doctrine para seguirem o padrão atual da documentação. Criação da rota /perfil, CRUD da entridade Perfil, desacoplado da entidade User. Utilização de colections, fieldsets, doctrine hydrator. A entidade Perfil foi totalmente modificada para o padrão da documentação do Doctrine.
</commit_message>
<xml_diff>
--- a/projeto.xlsx
+++ b/projeto.xlsx
@@ -823,8 +823,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G28" sqref="G25:G28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>